<commit_message>
Added Description column to the sheet
</commit_message>
<xml_diff>
--- a/Models_versioning.xlsx
+++ b/Models_versioning.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t xml:space="preserve">Sno</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">Model</t>
   </si>
   <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
     <t xml:space="preserve">Optimizer</t>
   </si>
   <si>
@@ -68,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">resnet18-pretrained, 512-128 linear, relu, 128-5 linear, softmax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pretrained  model weights, fc layer alone trained</t>
   </si>
   <si>
     <t xml:space="preserve">Adam</t>
@@ -241,32 +247,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="2" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.18367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.3928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="2" width="10.6632653061225"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -309,93 +316,102 @@
       <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="58.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I2" s="4" t="n">
+      <c r="J2" s="4" t="n">
         <v>0.0001</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="67.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="1" t="n">
+      <c r="H3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I3" s="4" t="n">
+      <c r="J3" s="4" t="n">
         <v>0.0004</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added metrics of Resnet18_imagenet_full model to sheet
</commit_message>
<xml_diff>
--- a/Models_versioning.xlsx
+++ b/Models_versioning.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t xml:space="preserve">Sno</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t xml:space="preserve">NLLLoss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RandomResizedCrop(300)</t>
   </si>
   <si>
     <t xml:space="preserve">imagenet_normalise </t>
@@ -127,6 +130,21 @@
   </si>
   <si>
     <t xml:space="preserve">[0.79111, 0.71371, 0.68229]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R18_imagenet_full</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pretrained  model weights, all layers trained</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.69351, 0.59728, 0.45618]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.75349, 0.82322, 0.84584]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.67943, 0.52374, 0.44371]</t>
   </si>
 </sst>
 </file>
@@ -247,30 +265,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="O5" activeCellId="0" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.3928571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.91326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.9438775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="2" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -320,7 +338,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
@@ -339,11 +357,11 @@
       <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="1" t="n">
-        <v>300</v>
+      <c r="G2" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I2" s="1" t="n">
         <v>5</v>
@@ -352,27 +370,27 @@
         <v>0.0001</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="67.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
@@ -386,11 +404,11 @@
       <c r="F3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="1" t="n">
-        <v>300</v>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>3</v>
@@ -399,19 +417,66 @@
         <v>0.0004</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="I4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J4" s="4" t="n">
+        <v>0.0004</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>32</v>
+      <c r="M4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
R18_imagenet_v2 - R18 fc layer with pretrained weights and image sizeof 448; cv score of ~0.75425
</commit_message>
<xml_diff>
--- a/Models_versioning.xlsx
+++ b/Models_versioning.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
   <si>
     <t xml:space="preserve">Sno</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">val_accuracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time taken (minutes)</t>
   </si>
   <si>
     <t xml:space="preserve">R18_imagenet</t>
@@ -145,6 +148,21 @@
   </si>
   <si>
     <t xml:space="preserve">[0.67943, 0.52374, 0.44371]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R18_imagenet_v2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RandomResizedCrop(448)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.95946, 0.74856, 0.68570]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.69729, 0.74860, 0.77215]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.75425, 0.66836, 0.63191]</t>
   </si>
 </sst>
 </file>
@@ -265,33 +283,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O5" activeCellId="0" sqref="O5"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.9438775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="2" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="2" width="10.2602040816327"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -336,6 +354,9 @@
       </c>
       <c r="O1" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -343,25 +364,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I2" s="1" t="n">
         <v>5</v>
@@ -370,19 +391,22 @@
         <v>0.0001</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -390,25 +414,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>3</v>
@@ -417,19 +441,22 @@
         <v>0.0004</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="P3" s="2" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -437,25 +464,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I4" s="1" t="n">
         <v>3</v>
@@ -464,19 +491,72 @@
         <v>0.0004</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P4" s="2" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="I5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J5" s="4" t="n">
+        <v>0.0004</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>38</v>
+      <c r="L5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P5" s="2" t="n">
+        <v>20.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>